<commit_message>
added viz.py, rreduced dicitionary, added full dictionary, updated clustering.py, modeling.py, prepare,py, kan's working notebook, report.
</commit_message>
<xml_diff>
--- a/zillow_data_dictionary.xlsx
+++ b/zillow_data_dictionary.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhe/zdabh/kaggle/published_to_kaggle/kaggle_publish_history/2017-05-04/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kanieladenis/codeup-data-science/zillow_clustering_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34880BE8-443B-3A4D-B3D8-AAA4099CE24F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16900" yWindow="-20780" windowWidth="27600" windowHeight="15880"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27600" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="5" r:id="rId1"/>
@@ -24,23 +25,23 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">PropertyLandUseTypeID!$A$1:$B$26</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="206">
   <si>
     <t>StoryTypeID</t>
   </si>
@@ -348,66 +349,24 @@
     <t xml:space="preserve"> Overall assessment of condition of the building from best (lowest) to worst (highest)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Number of bathrooms in home including fractional bathroom</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Number of 3/4 bathrooms in house (shower + sink + toilet)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Size of the finished living area on the first (entry) floor of the home</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Number of fireplaces in a home (if any)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Number of full bathrooms (sink, shower + bathtub, and toilet) present in home</t>
   </si>
   <si>
-    <t xml:space="preserve"> Total number of garages on the lot including an attached garage</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Type of home heating system</t>
   </si>
   <si>
     <t xml:space="preserve"> Latitude of the middle of the parcel multiplied by 10e6</t>
   </si>
   <si>
-    <t xml:space="preserve"> Number of stories or levels the home has</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Unique identifier for parcels (lots) </t>
   </si>
   <si>
     <t xml:space="preserve"> Number of pools on the lot (if any)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Total square footage of all pools on property</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Spa or Hot Tub</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pool with Spa/Hot Tub</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pool without hot tub</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> County land use code i.e. it's zoning at the county level</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Type of land use the property is zoned for</t>
   </si>
   <si>
-    <t xml:space="preserve"> Description of the allowed land uses (zoning) for that property</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> City in which the property is located (if any)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Zip code in which the property is located</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Total number of rooms in the principal residence</t>
   </si>
   <si>
@@ -423,12 +382,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Patio in  yard</t>
-  </si>
-  <si>
-    <t>Storage shed/building in yard</t>
-  </si>
-  <si>
     <t>The total tax assessed value of the parcel</t>
   </si>
   <si>
@@ -579,15 +532,6 @@
     <t>Residential Vacant Land</t>
   </si>
   <si>
-    <t>Type of deck (if any) present on parcel</t>
-  </si>
-  <si>
-    <t>County in which the property is located</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> What type of construction material was used to construct the home</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Architectural style of the home (i.e. ranch, colonial, split-level, etc…)</t>
   </si>
   <si>
@@ -597,21 +541,12 @@
     <t xml:space="preserve"> Type of floors in a multi-story house (i.e. basement and main level, split-level, attic, etc.).  See tab for details.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Does the home have a hot tub or spa</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Total number of square feet of all garages on lot including an attached garage</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Area of the lot in square feet</t>
   </si>
   <si>
     <t xml:space="preserve"> Census tract and block ID combined - also contains blockgroup assignment by extension</t>
   </si>
   <si>
-    <t xml:space="preserve"> Is a fireplace present in this home </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Longitude of the middle of the parcel multiplied by 10e6</t>
   </si>
   <si>
@@ -621,9 +556,6 @@
     <t>The total property tax assessed for that assessment year</t>
   </si>
   <si>
-    <t xml:space="preserve">The year of the property tax assessment </t>
-  </si>
-  <si>
     <t>BuildingClassTypeID</t>
   </si>
   <si>
@@ -645,36 +577,12 @@
     <t>Specialized buildings that do not fit in any of the above categories</t>
   </si>
   <si>
-    <t>Neighborhood in which the property is located</t>
-  </si>
-  <si>
-    <t>Base unfinished and finished area</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Calculated total finished living area of the home </t>
   </si>
   <si>
-    <t>Property taxes for this parcel are past due as of 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year for which the unpaid propert taxes were due </t>
-  </si>
-  <si>
     <t xml:space="preserve">The building framing type (steel frame, wood frame, concrete/brick) </t>
   </si>
   <si>
-    <t>Finished living area</t>
-  </si>
-  <si>
-    <t>Perimeter  living area</t>
-  </si>
-  <si>
-    <t>Total area</t>
-  </si>
-  <si>
-    <t>'taxdelinquencyyear'</t>
-  </si>
-  <si>
     <t>'airconditioningtypeid'</t>
   </si>
   <si>
@@ -696,57 +604,15 @@
     <t>'buildingclasstypeid'</t>
   </si>
   <si>
-    <t>'calculatedbathnbr'</t>
-  </si>
-  <si>
-    <t>'decktypeid'</t>
-  </si>
-  <si>
-    <t>'threequarterbathnbr'</t>
-  </si>
-  <si>
-    <t>'finishedfloor1squarefeet'</t>
-  </si>
-  <si>
     <t>'calculatedfinishedsquarefeet'</t>
   </si>
   <si>
-    <t>'finishedsquarefeet6'</t>
-  </si>
-  <si>
-    <t>'finishedsquarefeet12'</t>
-  </si>
-  <si>
-    <t>'finishedsquarefeet13'</t>
-  </si>
-  <si>
-    <t>'finishedsquarefeet15'</t>
-  </si>
-  <si>
-    <t>'finishedsquarefeet50'</t>
-  </si>
-  <si>
     <t>'fips'</t>
   </si>
   <si>
-    <t>'fireplacecnt'</t>
-  </si>
-  <si>
-    <t>'fireplaceflag'</t>
-  </si>
-  <si>
     <t>'fullbathcnt'</t>
   </si>
   <si>
-    <t>'garagecarcnt'</t>
-  </si>
-  <si>
-    <t>'garagetotalsqft'</t>
-  </si>
-  <si>
-    <t>'hashottuborspa'</t>
-  </si>
-  <si>
     <t>'heatingorsystemtypeid'</t>
   </si>
   <si>
@@ -759,72 +625,27 @@
     <t>'lotsizesquarefeet'</t>
   </si>
   <si>
-    <t>'numberofstories'</t>
-  </si>
-  <si>
     <t>'parcelid'</t>
   </si>
   <si>
     <t>'poolcnt'</t>
   </si>
   <si>
-    <t>'poolsizesum'</t>
-  </si>
-  <si>
-    <t>'pooltypeid10'</t>
-  </si>
-  <si>
-    <t>'pooltypeid2'</t>
-  </si>
-  <si>
-    <t>'pooltypeid7'</t>
-  </si>
-  <si>
-    <t>'propertycountylandusecode'</t>
-  </si>
-  <si>
     <t>'propertylandusetypeid'</t>
   </si>
   <si>
-    <t>'propertyzoningdesc'</t>
-  </si>
-  <si>
-    <t>'rawcensustractandblock'</t>
-  </si>
-  <si>
     <t>'censustractandblock'</t>
   </si>
   <si>
-    <t>'regionidcounty'</t>
-  </si>
-  <si>
-    <t>'regionidcity'</t>
-  </si>
-  <si>
-    <t>'regionidzip'</t>
-  </si>
-  <si>
-    <t>'regionidneighborhood'</t>
-  </si>
-  <si>
     <t>'roomcnt'</t>
   </si>
   <si>
     <t>'storytypeid'</t>
   </si>
   <si>
-    <t>'typeconstructiontypeid'</t>
-  </si>
-  <si>
     <t>'unitcnt'</t>
   </si>
   <si>
-    <t>'yardbuildingsqft17'</t>
-  </si>
-  <si>
-    <t>'yardbuildingsqft26'</t>
-  </si>
-  <si>
     <t>'yearbuilt'</t>
   </si>
   <si>
@@ -838,18 +659,12 @@
   </si>
   <si>
     <t>'taxamount'</t>
-  </si>
-  <si>
-    <t>'assessmentyear'</t>
-  </si>
-  <si>
-    <t>'taxdelinquencyflag'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1160,30 +975,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A28" activeCellId="9" sqref="A9:XFD9 A13:XFD13 A18:XFD18 A21:XFD21 A23:XFD23 A25:XFD25 A26:XFD26 A27:XFD27 A31:XFD31 A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.6640625" customWidth="1"/>
-    <col min="2" max="2" width="55.33203125" customWidth="1"/>
+    <col min="2" max="2" width="97.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>211</v>
+        <v>180</v>
       </c>
       <c r="B2" t="s">
         <v>98</v>
@@ -1191,15 +1006,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>181</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
         <v>99</v>
@@ -1207,7 +1022,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>183</v>
       </c>
       <c r="B5" t="s">
         <v>100</v>
@@ -1215,15 +1030,15 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>215</v>
+        <v>184</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>185</v>
       </c>
       <c r="B7" t="s">
         <v>101</v>
@@ -1231,418 +1046,162 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>217</v>
+        <v>186</v>
       </c>
       <c r="B8" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>218</v>
+        <v>187</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>219</v>
+        <v>188</v>
       </c>
       <c r="B10" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>220</v>
+        <v>189</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>221</v>
+        <v>190</v>
       </c>
       <c r="B12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>222</v>
+        <v>191</v>
       </c>
       <c r="B13" t="s">
-        <v>203</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>223</v>
+        <v>192</v>
       </c>
       <c r="B14" t="s">
-        <v>202</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>224</v>
+        <v>193</v>
       </c>
       <c r="B15" t="s">
-        <v>207</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="B16" t="s">
-        <v>208</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="B17" t="s">
-        <v>209</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>228</v>
+        <v>197</v>
       </c>
       <c r="B19" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>229</v>
+        <v>198</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>230</v>
+        <v>199</v>
       </c>
       <c r="B21" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>231</v>
+        <v>200</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>232</v>
+        <v>201</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>233</v>
+        <v>202</v>
       </c>
       <c r="B24" t="s">
-        <v>186</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="B25" t="s">
-        <v>185</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>236</v>
+        <v>205</v>
       </c>
       <c r="B27" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>237</v>
-      </c>
-      <c r="B28" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>238</v>
-      </c>
-      <c r="B29" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>239</v>
-      </c>
-      <c r="B30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>240</v>
-      </c>
-      <c r="B31" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>241</v>
-      </c>
-      <c r="B32" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>242</v>
-      </c>
-      <c r="B33" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>243</v>
-      </c>
-      <c r="B34" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>244</v>
-      </c>
-      <c r="B35" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>245</v>
-      </c>
-      <c r="B36" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>246</v>
-      </c>
-      <c r="B37" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>247</v>
-      </c>
-      <c r="B38" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>248</v>
-      </c>
-      <c r="B39" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>249</v>
-      </c>
-      <c r="B40" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>250</v>
-      </c>
-      <c r="B41" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>251</v>
-      </c>
-      <c r="B42" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>252</v>
-      </c>
-      <c r="B43" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>253</v>
-      </c>
-      <c r="B44" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>254</v>
-      </c>
-      <c r="B45" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>255</v>
-      </c>
-      <c r="B46" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>256</v>
-      </c>
-      <c r="B47" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>257</v>
-      </c>
-      <c r="B48" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>258</v>
-      </c>
-      <c r="B49" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>259</v>
-      </c>
-      <c r="B50" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>260</v>
-      </c>
-      <c r="B51" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>261</v>
-      </c>
-      <c r="B52" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>262</v>
-      </c>
-      <c r="B53" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>263</v>
-      </c>
-      <c r="B54" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>264</v>
-      </c>
-      <c r="B55" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>265</v>
-      </c>
-      <c r="B56" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>266</v>
-      </c>
-      <c r="B57" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>267</v>
-      </c>
-      <c r="B58" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>210</v>
-      </c>
-      <c r="B59" t="s">
-        <v>205</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1651,7 +1210,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1662,10 +1221,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1673,7 +1232,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1689,7 +1248,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1697,7 +1256,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1705,7 +1264,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1713,7 +1272,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1721,7 +1280,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1729,7 +1288,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1745,7 +1304,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1753,7 +1312,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1761,7 +1320,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1785,7 +1344,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1801,7 +1360,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1809,7 +1368,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1817,7 +1376,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1825,7 +1384,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1833,7 +1392,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1841,7 +1400,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1849,7 +1408,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1865,7 +1424,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1874,7 +1433,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1889,10 +1448,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="B1" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1900,7 +1459,7 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1908,7 +1467,7 @@
         <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1916,7 +1475,7 @@
         <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1924,7 +1483,7 @@
         <v>246</v>
       </c>
       <c r="B5" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1932,7 +1491,7 @@
         <v>247</v>
       </c>
       <c r="B6" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1940,7 +1499,7 @@
         <v>248</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1948,7 +1507,7 @@
         <v>260</v>
       </c>
       <c r="B8" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1956,7 +1515,7 @@
         <v>261</v>
       </c>
       <c r="B9" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1964,7 +1523,7 @@
         <v>262</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1972,7 +1531,7 @@
         <v>263</v>
       </c>
       <c r="B11" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1980,7 +1539,7 @@
         <v>264</v>
       </c>
       <c r="B12" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1988,7 +1547,7 @@
         <v>265</v>
       </c>
       <c r="B13" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1996,7 +1555,7 @@
         <v>266</v>
       </c>
       <c r="B14" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -2004,7 +1563,7 @@
         <v>267</v>
       </c>
       <c r="B15" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -2012,7 +1571,7 @@
         <v>268</v>
       </c>
       <c r="B16" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -2020,7 +1579,7 @@
         <v>269</v>
       </c>
       <c r="B17" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -2028,7 +1587,7 @@
         <v>270</v>
       </c>
       <c r="B18" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -2036,7 +1595,7 @@
         <v>271</v>
       </c>
       <c r="B19" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -2052,7 +1611,7 @@
         <v>274</v>
       </c>
       <c r="B21" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -2060,7 +1619,7 @@
         <v>275</v>
       </c>
       <c r="B22" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -2068,7 +1627,7 @@
         <v>276</v>
       </c>
       <c r="B23" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -2076,7 +1635,7 @@
         <v>279</v>
       </c>
       <c r="B24" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -2084,7 +1643,7 @@
         <v>290</v>
       </c>
       <c r="B25" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -2092,7 +1651,7 @@
         <v>291</v>
       </c>
       <c r="B26" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2101,7 +1660,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2404,7 +1963,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2531,7 +2090,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -2770,7 +2329,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2937,7 +2496,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2950,10 +2509,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="B1" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2961,7 +2520,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2969,7 +2528,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2977,7 +2536,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2985,7 +2544,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2993,7 +2552,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>